<commit_message>
[VL-2] All works :)
</commit_message>
<xml_diff>
--- a/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
+++ b/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\IdeaProjects\video-library\video-library-adapter\xlsx-adapter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C492567A-39A6-4F3A-8B5C-F0A4481737B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE7BD1-D08F-4BD7-9256-E066B59CC37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4153,8 +4153,8 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G13" sqref="G13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[VL-12] Make saveAll working on xlsx
</commit_message>
<xml_diff>
--- a/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
+++ b/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\IdeaProjects\video-library\video-library-adapter\xlsx-adapter\src\test\resources\"/>
     </mc:Choice>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="968">
   <si>
     <t>Titolo:</t>
   </si>
@@ -2940,6 +2940,9 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>3000</t>
   </si>
 </sst>
 </file>
@@ -4182,33 +4185,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="48" style="87" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.5546875" style="87" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.88671875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" style="5" customWidth="1"/>
-    <col min="20" max="20" width="18.6640625" style="5" customWidth="1"/>
-    <col min="21" max="21" width="18.6640625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" style="5" customWidth="1"/>
-    <col min="23" max="23" width="18.6640625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="18.6640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="18.6640625" customWidth="1"/>
-    <col min="27" max="27" width="18.6640625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="87" width="48.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="9.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="87" width="40.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="9.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="21.5546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="26.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="21.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.33203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="9.33203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="14.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="3" width="18.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="2" width="16.109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="5" width="12.6640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="5" width="18.6640625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="5" width="12.6640625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="5" width="18.6640625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="5" width="12.6640625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4377,8 +4380,8 @@
       <c r="B4" s="85" t="s">
         <v>925</v>
       </c>
-      <c r="C4" s="27">
-        <v>2007</v>
+      <c r="C4" s="27" t="n">
+        <v>2007.0</v>
       </c>
       <c r="D4" s="24">
         <v>10</v>
@@ -4457,8 +4460,8 @@
       <c r="B5" s="85" t="s">
         <v>926</v>
       </c>
-      <c r="C5" s="27">
-        <v>2009</v>
+      <c r="C5" s="27" t="n">
+        <v>2009.0</v>
       </c>
       <c r="D5" s="14">
         <v>8</v>
@@ -4535,8 +4538,8 @@
       <c r="B6" s="86" t="s">
         <v>250</v>
       </c>
-      <c r="C6" s="27">
-        <v>2011</v>
+      <c r="C6" s="27" t="n">
+        <v>2011.0</v>
       </c>
       <c r="D6" s="14">
         <v>7</v>
@@ -4607,8 +4610,8 @@
       <c r="B7" s="86" t="s">
         <v>266</v>
       </c>
-      <c r="C7" s="27">
-        <v>1962</v>
+      <c r="C7" s="27" t="n">
+        <v>1962.0</v>
       </c>
       <c r="D7" s="14">
         <v>10</v>
@@ -4709,23 +4712,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="8.109375" collapsed="true"/>
+    <col min="7" max="9" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="17" max="18" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6047,10 +6050,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="49.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -7488,13 +7491,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="124.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="53.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="48.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="124.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -12730,7 +12733,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[VL-12] Save also genres
</commit_message>
<xml_diff>
--- a/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
+++ b/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="975">
   <si>
     <t>Titolo:</t>
   </si>
@@ -2943,6 +2943,27 @@
   </si>
   <si>
     <t>3000</t>
+  </si>
+  <si>
+    <t>azione, commedia</t>
+  </si>
+  <si>
+    <t>avventura, azione, drammatico, fantascienza, storico, suspense/thriller</t>
+  </si>
+  <si>
+    <t>drammatico</t>
+  </si>
+  <si>
+    <t>avventura, azione, suspense/thriller</t>
+  </si>
+  <si>
+    <t>azione, guerra</t>
+  </si>
+  <si>
+    <t>avventura, azione, drammatico, fantascienza, suspense/thriller</t>
+  </si>
+  <si>
+    <t>commedia, romantico</t>
   </si>
 </sst>
 </file>
@@ -4378,16 +4399,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="85" t="s">
-        <v>925</v>
+        <v>967</v>
       </c>
       <c r="C4" s="27" t="n">
-        <v>2007.0</v>
+        <v>2018.0</v>
       </c>
       <c r="D4" s="24">
         <v>10</v>
       </c>
       <c r="E4" s="91" t="s">
-        <v>245</v>
+        <v>972</v>
       </c>
       <c r="F4" s="15">
         <v>8.1018518518518517E-2</v>
@@ -4467,7 +4488,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>270</v>
+        <v>973</v>
       </c>
       <c r="F5" s="15">
         <v>9.8935185185185182E-2</v>
@@ -4545,7 +4566,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>244</v>
+        <v>974</v>
       </c>
       <c r="F6" s="15">
         <v>7.075231481481481E-2</v>
@@ -4617,7 +4638,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>271</v>
+        <v>971</v>
       </c>
       <c r="F7" s="15">
         <v>7.3055555555555554E-2</v>

</xml_diff>

<commit_message>
[VL-12] Improve test part 2
</commit_message>
<xml_diff>
--- a/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
+++ b/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="977">
   <si>
     <t>Titolo:</t>
   </si>
@@ -2964,6 +2964,12 @@
   </si>
   <si>
     <t>commedia, romantico</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -4197,7 +4203,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
@@ -4393,306 +4399,6 @@
       <c r="AC3" s="83" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="85" t="s">
-        <v>967</v>
-      </c>
-      <c r="C4" s="27" t="n">
-        <v>2018.0</v>
-      </c>
-      <c r="D4" s="24">
-        <v>10</v>
-      </c>
-      <c r="E4" s="91" t="s">
-        <v>972</v>
-      </c>
-      <c r="F4" s="15">
-        <v>8.1018518518518517E-2</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="H4" s="13">
-        <v>25</v>
-      </c>
-      <c r="I4" s="11">
-        <v>1800</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="K4" s="14">
-        <v>640</v>
-      </c>
-      <c r="L4" s="14">
-        <v>48</v>
-      </c>
-      <c r="M4" s="24">
-        <v>6</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="O4" s="10">
-        <f>1.98*1024</f>
-        <v>2027.52</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="141">
-        <v>1</v>
-      </c>
-      <c r="S4" s="22">
-        <v>2012</v>
-      </c>
-      <c r="T4" s="67"/>
-      <c r="U4" s="143">
-        <v>2</v>
-      </c>
-      <c r="V4" s="23">
-        <v>41594</v>
-      </c>
-      <c r="W4" s="70" t="s">
-        <v>269</v>
-      </c>
-      <c r="X4" s="143"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="65"/>
-      <c r="AA4" s="141">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="26">
-        <v>44542</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>2</v>
-      </c>
-      <c r="B5" s="85" t="s">
-        <v>926</v>
-      </c>
-      <c r="C5" s="27" t="n">
-        <v>2009.0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>8</v>
-      </c>
-      <c r="E5" s="92" t="s">
-        <v>973</v>
-      </c>
-      <c r="F5" s="15">
-        <v>9.8935185185185182E-2</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="13">
-        <v>25</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1209</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="K5" s="14">
-        <v>128</v>
-      </c>
-      <c r="L5" s="14">
-        <v>48</v>
-      </c>
-      <c r="M5" s="14">
-        <v>2</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="O5" s="10">
-        <f>1.34*1024</f>
-        <v>1372.16</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="R5" s="141">
-        <v>4</v>
-      </c>
-      <c r="S5" s="17">
-        <v>2012</v>
-      </c>
-      <c r="T5" s="69"/>
-      <c r="U5" s="11">
-        <v>5</v>
-      </c>
-      <c r="V5" s="18">
-        <v>41538</v>
-      </c>
-      <c r="W5" s="18"/>
-      <c r="X5" s="14">
-        <v>6</v>
-      </c>
-      <c r="Y5" s="18">
-        <v>41886</v>
-      </c>
-      <c r="Z5" s="66" t="s">
-        <v>265</v>
-      </c>
-      <c r="AA5" s="141"/>
-    </row>
-    <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>3</v>
-      </c>
-      <c r="B6" s="86" t="s">
-        <v>250</v>
-      </c>
-      <c r="C6" s="27" t="n">
-        <v>2011.0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>7</v>
-      </c>
-      <c r="E6" s="92" t="s">
-        <v>974</v>
-      </c>
-      <c r="F6" s="15">
-        <v>7.075231481481481E-2</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="13">
-        <v>25</v>
-      </c>
-      <c r="I6" s="11">
-        <v>807</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="K6" s="14">
-        <v>128</v>
-      </c>
-      <c r="L6" s="14">
-        <v>48</v>
-      </c>
-      <c r="M6" s="14">
-        <v>2</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="O6" s="10">
-        <v>689</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>874</v>
-      </c>
-      <c r="R6" s="141">
-        <v>7</v>
-      </c>
-      <c r="S6" s="17">
-        <v>2012</v>
-      </c>
-      <c r="T6" s="69"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="66"/>
-      <c r="AA6" s="141">
-        <v>8</v>
-      </c>
-      <c r="AB6" s="26">
-        <v>44549</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>4</v>
-      </c>
-      <c r="B7" s="86" t="s">
-        <v>266</v>
-      </c>
-      <c r="C7" s="27" t="n">
-        <v>1962.0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>10</v>
-      </c>
-      <c r="E7" s="92" t="s">
-        <v>971</v>
-      </c>
-      <c r="F7" s="15">
-        <v>7.3055555555555554E-2</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="13">
-        <v>25</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1823</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="K7" s="14">
-        <v>128</v>
-      </c>
-      <c r="L7" s="14">
-        <v>48</v>
-      </c>
-      <c r="M7" s="14">
-        <v>2</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="O7" s="10">
-        <f>1.43*1024</f>
-        <v>1464.32</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>888</v>
-      </c>
-      <c r="R7" s="141"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="11">
-        <v>9</v>
-      </c>
-      <c r="V7" s="18">
-        <v>41565</v>
-      </c>
-      <c r="W7" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="141"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:Z7" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
[VL-12] Refactor part 1
</commit_message>
<xml_diff>
--- a/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
+++ b/video-library-adapter/xlsx-adapter/src/test/resources/TestCatalogoFilm.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="975">
   <si>
     <t>Titolo:</t>
   </si>
@@ -2964,12 +2964,6 @@
   </si>
   <si>
     <t>commedia, romantico</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -4203,7 +4197,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
@@ -4399,6 +4393,306 @@
       <c r="AC3" s="83" t="s">
         <v>965</v>
       </c>
+    </row>
+    <row r="4" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>967</v>
+      </c>
+      <c r="C4" s="27" t="n">
+        <v>2018.0</v>
+      </c>
+      <c r="D4" s="24">
+        <v>10</v>
+      </c>
+      <c r="E4" s="91" t="s">
+        <v>972</v>
+      </c>
+      <c r="F4" s="15">
+        <v>8.1018518518518517E-2</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="H4" s="13">
+        <v>25</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1800</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="K4" s="14">
+        <v>640</v>
+      </c>
+      <c r="L4" s="14">
+        <v>48</v>
+      </c>
+      <c r="M4" s="24">
+        <v>6</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="O4" s="10">
+        <f>1.98*1024</f>
+        <v>2027.52</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="141">
+        <v>1</v>
+      </c>
+      <c r="S4" s="22">
+        <v>2012</v>
+      </c>
+      <c r="T4" s="67"/>
+      <c r="U4" s="143">
+        <v>2</v>
+      </c>
+      <c r="V4" s="23">
+        <v>41594</v>
+      </c>
+      <c r="W4" s="70" t="s">
+        <v>269</v>
+      </c>
+      <c r="X4" s="143"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="65"/>
+      <c r="AA4" s="141">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="26">
+        <v>44542</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>926</v>
+      </c>
+      <c r="C5" s="27" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="D5" s="14">
+        <v>8</v>
+      </c>
+      <c r="E5" s="92" t="s">
+        <v>973</v>
+      </c>
+      <c r="F5" s="15">
+        <v>9.8935185185185182E-2</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="13">
+        <v>25</v>
+      </c>
+      <c r="I5" s="11">
+        <v>1209</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="K5" s="14">
+        <v>128</v>
+      </c>
+      <c r="L5" s="14">
+        <v>48</v>
+      </c>
+      <c r="M5" s="14">
+        <v>2</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="O5" s="10">
+        <f>1.34*1024</f>
+        <v>1372.16</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="141">
+        <v>4</v>
+      </c>
+      <c r="S5" s="17">
+        <v>2012</v>
+      </c>
+      <c r="T5" s="69"/>
+      <c r="U5" s="11">
+        <v>5</v>
+      </c>
+      <c r="V5" s="18">
+        <v>41538</v>
+      </c>
+      <c r="W5" s="18"/>
+      <c r="X5" s="14">
+        <v>6</v>
+      </c>
+      <c r="Y5" s="18">
+        <v>41886</v>
+      </c>
+      <c r="Z5" s="66" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA5" s="141"/>
+    </row>
+    <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="27" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="D6" s="14">
+        <v>7</v>
+      </c>
+      <c r="E6" s="92" t="s">
+        <v>974</v>
+      </c>
+      <c r="F6" s="15">
+        <v>7.075231481481481E-2</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="13">
+        <v>25</v>
+      </c>
+      <c r="I6" s="11">
+        <v>807</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="K6" s="14">
+        <v>128</v>
+      </c>
+      <c r="L6" s="14">
+        <v>48</v>
+      </c>
+      <c r="M6" s="14">
+        <v>2</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="O6" s="10">
+        <v>689</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="R6" s="141">
+        <v>7</v>
+      </c>
+      <c r="S6" s="17">
+        <v>2012</v>
+      </c>
+      <c r="T6" s="69"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="66"/>
+      <c r="AA6" s="141">
+        <v>8</v>
+      </c>
+      <c r="AB6" s="26">
+        <v>44549</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" s="86" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="27" t="n">
+        <v>1962.0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>10</v>
+      </c>
+      <c r="E7" s="92" t="s">
+        <v>971</v>
+      </c>
+      <c r="F7" s="15">
+        <v>7.3055555555555554E-2</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="13">
+        <v>25</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1823</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="K7" s="14">
+        <v>128</v>
+      </c>
+      <c r="L7" s="14">
+        <v>48</v>
+      </c>
+      <c r="M7" s="14">
+        <v>2</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="O7" s="10">
+        <f>1.43*1024</f>
+        <v>1464.32</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>888</v>
+      </c>
+      <c r="R7" s="141"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="11">
+        <v>9</v>
+      </c>
+      <c r="V7" s="18">
+        <v>41565</v>
+      </c>
+      <c r="W7" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="66"/>
+      <c r="AA7" s="141"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:Z7" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>